<commit_message>
updated tasks and bayes inference spreadsheet
</commit_message>
<xml_diff>
--- a/excel_utilities/Расчет_условных_вероятностей_по_статистике.xlsx
+++ b/excel_utilities/Расчет_условных_вероятностей_по_статистике.xlsx
@@ -1,25 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rnt\decision_tree_examples\excel_utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rnt\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F921320-8A28-4D8C-B572-C0339C60617C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118749A9-1483-47DC-A15C-99515E45CE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29520" yWindow="-3612" windowWidth="20736" windowHeight="13848" xr2:uid="{2AF16E1D-46D8-4F6C-8442-72B2259B6037}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{2AF16E1D-46D8-4F6C-8442-72B2259B6037}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Расчет по Байесу" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="P_A_B">Лист1!#REF!</definedName>
-    <definedName name="P_A_B1">Лист1!#REF!</definedName>
-    <definedName name="P_B">Лист1!#REF!</definedName>
-    <definedName name="P_B1">Лист1!#REF!</definedName>
+    <definedName name="P_A_B" localSheetId="0">'Расчет по Байесу'!#REF!</definedName>
+    <definedName name="P_A_B">#REF!</definedName>
+    <definedName name="P_A_B1" localSheetId="0">'Расчет по Байесу'!#REF!</definedName>
+    <definedName name="P_A_B1">#REF!</definedName>
+    <definedName name="P_B" localSheetId="0">'Расчет по Байесу'!#REF!</definedName>
+    <definedName name="P_B">#REF!</definedName>
+    <definedName name="P_B1" localSheetId="0">'Расчет по Байесу'!#REF!</definedName>
+    <definedName name="P_B1">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
   <si>
     <t>P(B)</t>
   </si>
@@ -87,22 +91,16 @@
     <t>1. Исходные данные -статистика успешности исследований</t>
   </si>
   <si>
-    <t>2. Расчет совместных вероятностей</t>
-  </si>
-  <si>
-    <t>3. Расчет условный вероятностей</t>
-  </si>
-  <si>
-    <t>Совместная вероятность A и B</t>
-  </si>
-  <si>
-    <t>Вероятность B</t>
-  </si>
-  <si>
-    <t>Вероятность A</t>
-  </si>
-  <si>
-    <t>Условная вероятность А при условии B</t>
+    <t>2. Расчет условных вероятностей при известной геологии Р(B|A)</t>
+  </si>
+  <si>
+    <t>Априорная оценка геологии Р(А)</t>
+  </si>
+  <si>
+    <t>3. Расчет вероятности заключения отчета Р(В)</t>
+  </si>
+  <si>
+    <t>4. Расчет условных вероятностей Р(В|A)</t>
   </si>
 </sst>
 </file>
@@ -159,7 +157,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -233,19 +231,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -299,17 +284,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -381,20 +355,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -406,60 +397,22 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -479,68 +432,25 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>523461</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>94801</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>154672</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>549967</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>71894</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Рисунок 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13F2993E-9F7B-4076-AE5C-4AE97C459D2E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect l="6234" t="14783" r="4252" b="10275"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4406348" y="4658140"/>
-          <a:ext cx="1855306" cy="636104"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>524787</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>181887</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>34457</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>75870</xdr:rowOff>
+      <xdr:colOff>257614</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>48656</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="Выноска: изогнутая линия с чертой 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{760FB7CC-1D44-4B8A-81DE-EAFDC6511548}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD18BF00-40D7-4B0F-B488-6ED7C903A01F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -548,8 +458,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4410987" y="2010687"/>
-          <a:ext cx="1338470" cy="259743"/>
+          <a:off x="4775658" y="2375358"/>
+          <a:ext cx="1469099" cy="264098"/>
         </a:xfrm>
         <a:prstGeom prst="accentCallout2">
           <a:avLst>
@@ -557,8 +467,8 @@
             <a:gd name="adj2" fmla="val -8333"/>
             <a:gd name="adj3" fmla="val 18750"/>
             <a:gd name="adj4" fmla="val -16667"/>
-            <a:gd name="adj5" fmla="val 254205"/>
-            <a:gd name="adj6" fmla="val -94349"/>
+            <a:gd name="adj5" fmla="val 101697"/>
+            <a:gd name="adj6" fmla="val -209571"/>
           </a:avLst>
         </a:prstGeom>
       </xdr:spPr>
@@ -679,7 +589,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1200"/>
-            <a:t>P(AB) = 1 / 30</a:t>
+            <a:t>P(B|A) = 6 / 10</a:t>
           </a:r>
           <a:endParaRPr lang="ru-RU" sz="1200"/>
         </a:p>
@@ -689,23 +599,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>521804</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>159121</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>92954</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>31474</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>139147</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>397328</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>32656</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Выноска: изогнутая линия с чертой 3">
+        <xdr:cNvPr id="5" name="Выноска: изогнутая линия с чертой 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3B3F7F8-7181-4F47-A0B7-88BE658CC62D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5879C17A-5A8D-4264-B9C6-45E8A67BCD78}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -713,8 +623,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4408004" y="3314700"/>
-          <a:ext cx="1338470" cy="322027"/>
+          <a:off x="4839978" y="3984597"/>
+          <a:ext cx="2850779" cy="304373"/>
         </a:xfrm>
         <a:prstGeom prst="accentCallout2">
           <a:avLst>
@@ -722,8 +632,8 @@
             <a:gd name="adj2" fmla="val -8333"/>
             <a:gd name="adj3" fmla="val 18750"/>
             <a:gd name="adj4" fmla="val -16667"/>
-            <a:gd name="adj5" fmla="val -10527"/>
-            <a:gd name="adj6" fmla="val -101789"/>
+            <a:gd name="adj5" fmla="val 70909"/>
+            <a:gd name="adj6" fmla="val -207522"/>
           </a:avLst>
         </a:prstGeom>
       </xdr:spPr>
@@ -844,15 +754,11 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1200"/>
-            <a:t>P(A) = </a:t>
+            <a:t>P(B) = 0.6</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="ru-RU" sz="1200"/>
-            <a:t>5</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200"/>
-            <a:t> / 30</a:t>
+            <a:rPr lang="en-US" sz="1200" baseline="0"/>
+            <a:t>*0.15 + 0.2*0.6 + 0.17 *0.25</a:t>
           </a:r>
           <a:endParaRPr lang="ru-RU" sz="1200"/>
         </a:p>
@@ -862,23 +768,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>523792</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>136498</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>171757</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>100148</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>33462</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>30481</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>191637</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>130629</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Выноска: изогнутая линия с чертой 4">
+        <xdr:cNvPr id="6" name="Выноска: изогнутая линия с чертой 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDA382B2-997A-4D56-960C-B463DBBEBC7A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEF21EAC-D7D4-44CA-9AC1-6BE881A3F470}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -886,8 +792,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4409992" y="2521558"/>
-          <a:ext cx="1338470" cy="259743"/>
+          <a:off x="4852614" y="5466805"/>
+          <a:ext cx="1979309" cy="220981"/>
         </a:xfrm>
         <a:prstGeom prst="accentCallout2">
           <a:avLst>
@@ -895,8 +801,8 @@
             <a:gd name="adj2" fmla="val -8333"/>
             <a:gd name="adj3" fmla="val 18750"/>
             <a:gd name="adj4" fmla="val -16667"/>
-            <a:gd name="adj5" fmla="val 70909"/>
-            <a:gd name="adj6" fmla="val -44507"/>
+            <a:gd name="adj5" fmla="val 144725"/>
+            <a:gd name="adj6" fmla="val -160981"/>
           </a:avLst>
         </a:prstGeom>
       </xdr:spPr>
@@ -1017,15 +923,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1200"/>
-            <a:t>P(B) = 1</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="ru-RU" sz="1200"/>
-            <a:t>0</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200"/>
-            <a:t> / 30</a:t>
+            <a:t>P(B|A) = 0.6*0.15 / 0.25</a:t>
           </a:r>
           <a:endParaRPr lang="ru-RU" sz="1200"/>
         </a:p>
@@ -1033,169 +931,96 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>547313</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>7619</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>567193</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>157036</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Выноска: изогнутая линия с чертой 5">
+        <xdr:cNvPr id="2049" name="AutoShape 1" descr="{\displaystyle P(A_{j}\mid B)={\frac {P(B\mid A_{j})P(A_{j})}{\sum _{i=1}^{N}P(B\mid A_{i})P(A_{i})}}}">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F21CC76A-D25B-4159-A240-B30DD3229785}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F1120C2-92FF-F713-EA7D-D3E561FBEEB9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
       </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7946571" y="2960914"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>517073</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>157843</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>35380</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Рисунок 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52CF0E9D-E5AF-B9CB-76AB-50F6FA4B2E13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4433513" y="4061459"/>
-          <a:ext cx="1848680" cy="332297"/>
+          <a:off x="9116787" y="342900"/>
+          <a:ext cx="4743450" cy="1066800"/>
         </a:xfrm>
-        <a:prstGeom prst="accentCallout2">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 18750"/>
-            <a:gd name="adj2" fmla="val -8333"/>
-            <a:gd name="adj3" fmla="val 18750"/>
-            <a:gd name="adj4" fmla="val -16667"/>
-            <a:gd name="adj5" fmla="val 73297"/>
-            <a:gd name="adj6" fmla="val -77935"/>
-          </a:avLst>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="ru-RU"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200"/>
-            <a:t>P(A|B) = 0.03 / 0.17</a:t>
-          </a:r>
-          <a:endParaRPr lang="ru-RU" sz="1200"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1497,39 +1322,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDA23D6-9429-413E-8810-B2C6E6ADE9AC}">
-  <sheetPr codeName="Лист1"/>
-  <dimension ref="A2:J27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42629B00-97A4-409E-ABFF-4616D88C4E39}">
+  <dimension ref="A2:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" customWidth="1"/>
-    <col min="3" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.53515625" customWidth="1"/>
+    <col min="3" max="6" width="10.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C4" s="4" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
       <c r="H4" t="s">
         <v>7</v>
       </c>
       <c r="I4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
         <v>1</v>
@@ -1547,9 +1374,14 @@
       <c r="I5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="K5" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A6" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1568,9 +1400,18 @@
         <f>SUM(C6:E6)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
+      <c r="K6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A7" s="23"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1581,15 +1422,25 @@
         <v>10</v>
       </c>
       <c r="E7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" ref="F7:F8" si="0">SUM(C7:E7)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="M7" s="3">
+        <f>1-L7-K7</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A8" s="23"/>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1607,7 +1458,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="2">
         <f>SUM(C6:C8)</f>
@@ -1619,31 +1470,26 @@
       </c>
       <c r="E9" s="2">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F9" s="2">
         <f>SUM(C9:E9)</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="4" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C13" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
         <v>1</v>
@@ -1651,237 +1497,242 @@
       <c r="D14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+    </row>
+    <row r="15" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="10">
-        <f>C6/$F$9</f>
+      <c r="C15" s="4">
+        <f>C6/C$9</f>
+        <v>0.6</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" ref="D15:E15" si="2">D6/D$9</f>
         <v>0.2</v>
       </c>
-      <c r="D15" s="10">
-        <f>D6/$F$9</f>
-        <v>0.1</v>
-      </c>
-      <c r="E15" s="18">
-        <f>E6/$F$9</f>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="F15" s="22">
-        <f>SUM(C15:E15)</f>
-        <v>0.33333333333333337</v>
-      </c>
-      <c r="J15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
+      <c r="E15" s="4">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A16" s="17"/>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="10">
-        <f>C7/$F$9</f>
+      <c r="C16" s="4">
+        <f t="shared" ref="C16:E17" si="3">C7/C$9</f>
+        <v>0.3</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="3"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="18"/>
+      <c r="B17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="4">
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="D16" s="10">
-        <f>D7/$F$9</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E16" s="18">
-        <f>E7/$F$9</f>
+      <c r="D17" s="4">
+        <f t="shared" si="3"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="7">
+        <f>SUM(C15:C17)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" ref="D18:E18" si="4">SUM(D15:D17)</f>
+        <v>1</v>
+      </c>
+      <c r="E18" s="8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B21" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C22" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
+    </row>
+    <row r="23" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="15">
+        <f>(C15*K7+D15*L7+E15*M7)</f>
+        <v>0.25166666666666665</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A24" s="17"/>
+      <c r="B24" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="15">
+        <f>(C16*K7+D16*L7+E16*M7)</f>
+        <v>0.48666666666666664</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A25" s="18"/>
+      <c r="B25" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="15">
+        <f>(C17*K7+D17*L7+E17*M7)</f>
+        <v>0.26166666666666666</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="14">
+        <f>SUM(C23:C25)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B28" s="24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C30" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F16" s="22">
-        <f t="shared" ref="F16:F17" si="2">SUM(C16:E16)</f>
-        <v>0.43333333333333335</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="9"/>
-      <c r="B17" s="12" t="s">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A32" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="4">
+        <f>C15*K$7/$C23</f>
+        <v>0.35761589403973509</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" ref="D32:E34" si="5">D15*L$7/$C23</f>
+        <v>0.47682119205298013</v>
+      </c>
+      <c r="E32" s="4">
+        <f t="shared" si="5"/>
+        <v>0.16556291390728478</v>
+      </c>
+      <c r="F32" s="11">
+        <f>SUM(C32:E32)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A33" s="17"/>
+      <c r="B33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="4">
+        <f t="shared" ref="C33:C34" si="6">C16*K$7/$C24</f>
+        <v>9.2465753424657543E-2</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" si="5"/>
+        <v>0.82191780821917804</v>
+      </c>
+      <c r="E33" s="4">
+        <f t="shared" si="5"/>
+        <v>8.5616438356164379E-2</v>
+      </c>
+      <c r="F33" s="11">
+        <f t="shared" ref="F33:F34" si="7">SUM(C33:E33)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="18"/>
+      <c r="B34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="13">
-        <f>C8/$F$9</f>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="D17" s="13">
-        <f>D8/$F$9</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="E17" s="19">
-        <f>E8/$F$9</f>
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="F17" s="23">
-        <f t="shared" si="2"/>
-        <v>0.23333333333333334</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="15">
-        <f>SUM(C15:C17)</f>
-        <v>0.33333333333333337</v>
-      </c>
-      <c r="D18" s="15">
-        <f t="shared" ref="D18" si="3">SUM(D15:D17)</f>
-        <v>0.5</v>
-      </c>
-      <c r="E18" s="16">
-        <f t="shared" ref="E18" si="4">SUM(E15:E17)</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="F18" s="20">
-        <f>SUM(C18:E18)</f>
+      <c r="C34" s="4">
+        <f t="shared" si="6"/>
+        <v>5.7324840764331211E-2</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" si="5"/>
+        <v>0.30573248407643316</v>
+      </c>
+      <c r="E34" s="4">
+        <f t="shared" si="5"/>
+        <v>0.63694267515923564</v>
+      </c>
+      <c r="F34" s="12">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="30"/>
-      <c r="E22" s="31"/>
-      <c r="H22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="17"/>
-      <c r="C23" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="F23" s="25" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="28">
-        <f>C15/C$18</f>
-        <v>0.6</v>
-      </c>
-      <c r="D24" s="28">
-        <f>D15/D$18</f>
-        <v>0.2</v>
-      </c>
-      <c r="E24" s="28">
-        <f>E15/E$18</f>
-        <v>0.2</v>
-      </c>
-      <c r="F24" s="11">
-        <f>SUM(C24:E24)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="28">
-        <f>C16/C$18</f>
-        <v>0.3</v>
-      </c>
-      <c r="D25" s="28">
-        <f>D16/D$18</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="E25" s="28">
-        <f>E16/E$18</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="11">
-        <f t="shared" ref="F25:F26" si="5">SUM(C25:E25)</f>
-        <v>0.96666666666666656</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="9"/>
-      <c r="B26" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="29">
-        <f>C17/C$18</f>
-        <v>9.9999999999999992E-2</v>
-      </c>
-      <c r="D26" s="29">
-        <f>D17/D$18</f>
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="E26" s="29">
-        <f>E17/E$18</f>
-        <v>0.8</v>
-      </c>
-      <c r="F26" s="11">
-        <f t="shared" si="5"/>
-        <v>1.0333333333333334</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="27">
-        <f>SUM(C24:C26)</f>
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="D27" s="27">
-        <f t="shared" ref="D27" si="6">SUM(D24:D26)</f>
-        <v>1</v>
-      </c>
-      <c r="E27" s="27">
-        <f t="shared" ref="E27" si="7">SUM(E24:E26)</f>
-        <v>1</v>
-      </c>
-      <c r="F27" s="6">
-        <f>SUM(C27:E27)</f>
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="A15:A17"/>
+  <mergeCells count="9">
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="A32:A34"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="C13:E13"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="A23:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>